<commit_message>
manual Task is updated
</commit_message>
<xml_diff>
--- a/ManualTask/TestCase.xlsx
+++ b/ManualTask/TestCase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>TC Number</t>
   </si>
@@ -34,6 +34,270 @@
   </si>
   <si>
     <t>Sevirity</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>*Chrome browser
+*Stable internet connection</t>
+  </si>
+  <si>
+    <t>*Open URL
+*Fill The First Name,
+LastName, Phone, Email, Password And Confirm Password</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>The Registration is done successfully
+*The Home Page is displayed</t>
+  </si>
+  <si>
+    <t>Validating Registaration 
+with Valid First Name</t>
+  </si>
+  <si>
+    <t>Validating Registaration 
+with inValid First Name</t>
+  </si>
+  <si>
+    <t>Validating Registaration 
+with inValid Last Name</t>
+  </si>
+  <si>
+    <t>Validating Registaration 
+with Last Name equals First Name</t>
+  </si>
+  <si>
+    <t>Validating Registaration 
+with invalid email</t>
+  </si>
+  <si>
+    <t>Error In the Registration,
+*Error Message "Invalid Email" is displayed</t>
+  </si>
+  <si>
+    <t>Error In the Registration,
+*Error Message "Invalid Last name " is displayed</t>
+  </si>
+  <si>
+    <t>Error In the Registration,
+*Error Message "Invalid Last name" is displayed</t>
+  </si>
+  <si>
+    <t>Error In the Registration,
+*Error Message "Invalid First name" is displayed</t>
+  </si>
+  <si>
+    <t>Validating Registaration 
+with allready registered email</t>
+  </si>
+  <si>
+    <t>Error In the Registration,
+*Error Message "This email is allready registered" is displayed</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor@gmail.com"
+*Password = "Noor%66"
+* Confirm Password "Noor%66"</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noorgmail.com"
+*Password = "Noor%66"
+* Confirm Password "Noor%66"</t>
+  </si>
+  <si>
+    <t>Error In the Registration,
+*Error Message "Invalid Password" is displayed</t>
+  </si>
+  <si>
+    <t>Validating Registaration 
+with with invalid Password
+ no spatial characters</t>
+  </si>
+  <si>
+    <t>Validating Registaration 
+with with invalid Password
+ no small letters</t>
+  </si>
+  <si>
+    <t>Validating Registaration 
+with with invalid Password
+ no capital letters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating Registaration 
+The Password is not equal
+confirm password
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validating Registaration 
+with very long Password
+</t>
+  </si>
+  <si>
+    <t>Regestration</t>
+  </si>
+  <si>
+    <t>Verification mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the validation mail is sent after registration
+</t>
+  </si>
+  <si>
+    <t>The Registration is done successfully
+*The Home Page is displayed
+*The validation mail is sent successfully.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the validation link in the validation mail
+</t>
+  </si>
+  <si>
+    <t>* First Name = "Nooran"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor13@gmail.com"
+*Password = "Noor%38789857934539465937498849466"
+* Confirm Password "Noor%38789857934539465937498849466"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* First Name = "Ola"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor14@gmail.com"
+*Password = "Noor%38789857934539465937498849466"
+* Confirm Password "Noor%38789857934539465937498849466"
+</t>
+  </si>
+  <si>
+    <t>*Open URL
+*Fill The First Name,
+LastName, Phone, Email, Password And Confirm Password
+*Open the mail
+*click on the validation link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Registration is done successfully
+*The Home Page is displayed
+</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor12@gmail.com"
+*Password = "Noor%38789857934539465937498849466"
+* Confirm Password "Noor%38789857934539465937498849466"</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor11@gmail.com"
+*Password = "Noor%66"
+* Confirm Password "Noor&amp;6666"</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor10@gmail.com"
+*Password = "Noor66"
+* Confirm Password "Noor66"</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor9@gmail.com"
+*Password = "NOOR%66"
+* Confirm Password "NOOR%66"</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor8@gmail.com"
+*Password = "noor%66"
+* Confirm Password ="noor%66"</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor6@gmail.com"
+*Password = "Noor%66"
+* Confirm Password "Noor%66"</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "Nehal"
+* Phone = "01028374659"
+* Email = "noor4@gmail.com"
+*Password = "Noor%66"
+* Confirm Password "Noor%66"</t>
+  </si>
+  <si>
+    <t>* First Name = "Nehal"
+*LastName = "srour"
+* Phone = "01028374659"
+* Email = "noor3@gmail.com"
+*Password = "Noor%66"
+* Confirm Password "Noor%66"</t>
+  </si>
+  <si>
+    <t>* First Name = "nehal"
+*LastName = "Srour"
+* Phone = "01028374659"
+* Email = "noor2@gmail.com"
+*Password = "Noor%66"
+* Confirm Password "Noor%66"</t>
+  </si>
+  <si>
+    <t>Login with valid email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+* Email = "noor14@gmail.com"
+*Password = "Noor%38789857934539465937498849466"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Open URL
+*Fill Email and Password 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Login is done successfully
+*The Home Page is displayed
+</t>
+  </si>
+  <si>
+    <t>Login with invalid email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+* Email = "noor3@gmail.com"
+*Password = "Noor%38789857934539465937498849466"
+</t>
+  </si>
+  <si>
+    <t>Error In Login
+*Error Message "This email not correct" is displayed</t>
   </si>
 </sst>
 </file>
@@ -88,10 +352,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -388,41 +660,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" customWidth="1"/>
+    <col min="7" max="7" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1"/>
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="31.8" customHeight="1">
+      <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="190.2" customHeight="1">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="31.8" customHeight="1">
+      <c r="E15" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="190.2" customHeight="1">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="2" customFormat="1" ht="190.2" customHeight="1">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="29.4" customHeight="1">
+      <c r="E18" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="2" customFormat="1" ht="181.2" customHeight="1">
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="2" customFormat="1" ht="181.2" customHeight="1">
+      <c r="A20" s="2">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="2" customFormat="1"/>
+    <row r="22" spans="1:7" s="2" customFormat="1"/>
+    <row r="23" spans="1:7" s="2" customFormat="1"/>
+    <row r="24" spans="1:7" s="2" customFormat="1"/>
+    <row r="25" spans="1:7" s="2" customFormat="1"/>
+    <row r="26" spans="1:7" s="2" customFormat="1"/>
+    <row r="27" spans="1:7" s="2" customFormat="1"/>
+    <row r="28" spans="1:7" s="2" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>